<commit_message>
Added all results from RTS/CTS tests
</commit_message>
<xml_diff>
--- a/new_results/scenario2/RTS_CTS_21_legacy/results.xlsx
+++ b/new_results/scenario2/RTS_CTS_21_legacy/results.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MetodySymulacyjne\MS_project2\new_results\scenario2\RTS_CTS_21_legacy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADE38C9-098C-4C7A-9075-1596C650321A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-23554" yWindow="-6523" windowWidth="23657" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ax" sheetId="1" r:id="rId1"/>
     <sheet name="legacy" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>Sta_num</t>
   </si>
@@ -35,6 +52,9 @@
     <t>333</t>
   </si>
   <si>
+    <t>334</t>
+  </si>
+  <si>
     <t>335</t>
   </si>
   <si>
@@ -47,8 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,17 +101,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -129,9 +157,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,9 +191,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +243,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -372,14 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,173 +462,487 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>398.9923477200001</v>
+        <v>611.06727751199992</v>
       </c>
       <c r="D2">
-        <v>6.333211868571428</v>
+        <v>9.6994805954285699</v>
       </c>
       <c r="E2">
+        <v>4.0158240746031746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>551.07998695999993</v>
+      </c>
+      <c r="D3">
+        <v>8.7473013803174613</v>
+      </c>
+      <c r="E3">
+        <v>4.4371252698412693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>626.13991317999989</v>
+      </c>
+      <c r="D4">
+        <v>9.9387287806349214</v>
+      </c>
+      <c r="E4">
+        <v>4.188029444444445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>579.71658816499985</v>
+      </c>
+      <c r="D5">
+        <v>9.2018506057936502</v>
+      </c>
+      <c r="E5">
+        <v>4.4632216666666658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>535.09476444000006</v>
+      </c>
+      <c r="D6">
+        <v>8.493567689523811</v>
+      </c>
+      <c r="E6">
+        <v>3.446235190476191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>489.14880297000002</v>
+      </c>
+      <c r="D7">
+        <v>7.7642667138095236</v>
+      </c>
+      <c r="E7">
+        <v>4.4111353968253963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>520.89275148000013</v>
+      </c>
+      <c r="D8">
+        <v>8.2681389123809534</v>
+      </c>
+      <c r="E8">
+        <v>4.501172968253969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>457.82929014999991</v>
+      </c>
+      <c r="D9">
+        <v>7.2671315896825392</v>
+      </c>
+      <c r="E9">
+        <v>3.7221408412698409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>488.27785319999998</v>
+      </c>
+      <c r="D10">
+        <v>7.7504421142857138</v>
+      </c>
+      <c r="E10">
+        <v>4.7460712222222234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>457.78240539999979</v>
+      </c>
+      <c r="D11">
+        <v>7.2663873873015881</v>
+      </c>
+      <c r="E11">
+        <v>4.2594664761904761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>489.70512021000002</v>
+      </c>
+      <c r="D12">
+        <v>7.7730971461904774</v>
+      </c>
+      <c r="E12">
+        <v>4.4716251809523806</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>398.99234772000011</v>
+      </c>
+      <c r="D13">
+        <v>6.3332118685714276</v>
+      </c>
+      <c r="E13">
         <v>3.852365219047619</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>349.5211178599998</v>
-      </c>
-      <c r="D3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>349.52111785999978</v>
+      </c>
+      <c r="D14">
         <v>5.547954251746031</v>
       </c>
-      <c r="E3">
-        <v>4.461754253968254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="E14">
+        <v>4.4617542539682544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>425.85943592</v>
-      </c>
-      <c r="D4">
-        <v>6.759673586031745</v>
-      </c>
-      <c r="E4">
-        <v>4.769441904761904</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>425.85943592000001</v>
+      </c>
+      <c r="D15">
+        <v>6.7596735860317452</v>
+      </c>
+      <c r="E15">
+        <v>4.7694419047619041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>428.0883993700002</v>
-      </c>
-      <c r="D5">
-        <v>6.795053958253969</v>
-      </c>
-      <c r="E5">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>428.08839937000022</v>
+      </c>
+      <c r="D16">
+        <v>6.7950539582539689</v>
+      </c>
+      <c r="E16">
         <v>4.429266873015874</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>40.754125000000002</v>
+      </c>
+      <c r="D1">
+        <v>5.8220178571428578</v>
+      </c>
+      <c r="E1">
+        <v>4.3585857142857138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>35.415648089999991</v>
+      </c>
+      <c r="D2">
+        <v>5.0593782985714268</v>
+      </c>
+      <c r="E2">
+        <v>4.1468557142857154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>54.544483999999997</v>
+      </c>
+      <c r="D3">
+        <v>7.7920691428571427</v>
+      </c>
+      <c r="E3">
+        <v>4.2416471428571434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>67.463042424000008</v>
+      </c>
+      <c r="D4">
+        <v>4.818788744571429</v>
+      </c>
+      <c r="E4">
+        <v>4.9527299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>71.931100000000001</v>
+      </c>
+      <c r="D5">
+        <v>5.1379357142857147</v>
+      </c>
+      <c r="E5">
+        <v>5.0155035714285727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>75.606069000000005</v>
+      </c>
+      <c r="D6">
+        <v>5.4004335000000001</v>
+      </c>
+      <c r="E6">
+        <v>4.9770457142857154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>60.885220060000002</v>
+      </c>
+      <c r="D7">
+        <v>4.3489442900000004</v>
+      </c>
+      <c r="E7">
+        <v>4.4028896928571433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>117.45091995</v>
+      </c>
+      <c r="D8">
+        <v>5.5929009499999998</v>
+      </c>
+      <c r="E8">
+        <v>3.9834104761904761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>117.56355963</v>
+      </c>
+      <c r="D9">
+        <v>5.5982647442857152</v>
+      </c>
+      <c r="E9">
+        <v>5.3596314285714284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>94.295313010000015</v>
+      </c>
+      <c r="D10">
+        <v>4.4902530004761907</v>
+      </c>
+      <c r="E10">
+        <v>4.7395833809523813</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>65.668271300000001</v>
+      </c>
+      <c r="D11">
+        <v>3.1270605380952379</v>
+      </c>
+      <c r="E11">
+        <v>4.1907789999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>117.45091995</v>
-      </c>
-      <c r="D2">
-        <v>5.59290095</v>
-      </c>
-      <c r="E2">
-        <v>3.983410476190476</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>117.56355963</v>
-      </c>
-      <c r="D3">
-        <v>5.598264744285715</v>
-      </c>
-      <c r="E3">
-        <v>5.359631428571428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>94.29531301000002</v>
-      </c>
-      <c r="D4">
-        <v>4.490253000476191</v>
-      </c>
-      <c r="E4">
-        <v>4.739583380952381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>65.6682713</v>
-      </c>
-      <c r="D5">
-        <v>3.127060538095238</v>
-      </c>
-      <c r="E5">
-        <v>4.190778999999999</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>